<commit_message>
fix the supplier import
</commit_message>
<xml_diff>
--- a/LUSSISADTeam10Web/Content/test1.xlsx
+++ b/LUSSISADTeam10Web/Content/test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AD_Documents\supplier csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{156734A6-1F4A-4A2C-94B0-5EF8E038C06D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0ECCD68-1038-43E9-943D-878DEFBBAFDD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9660" xr2:uid="{9E7BC6C7-8E8A-4B7C-8FE3-67E2C8BF1C74}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>SupId</t>
   </si>
@@ -60,10 +60,7 @@
     <t>each</t>
   </si>
   <si>
-    <t>Ruler</t>
-  </si>
-  <si>
-    <t>Pencil</t>
+    <t xml:space="preserve">Exercise Book A4 Hardcover(150pg) </t>
   </si>
 </sst>
 </file>
@@ -418,13 +415,13 @@
   <dimension ref="C4:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="24.109375" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="6" max="6" width="48.5546875" customWidth="1"/>
     <col min="7" max="8" width="5.109375" customWidth="1"/>
     <col min="9" max="9" width="12.44140625" customWidth="1"/>
   </cols>
@@ -466,7 +463,7 @@
         <v>9</v>
       </c>
       <c r="G5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -483,19 +480,19 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H6" t="s">
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the excel file import api method
</commit_message>
<xml_diff>
--- a/LUSSISADTeam10Web/Content/test1.xlsx
+++ b/LUSSISADTeam10Web/Content/test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AD_Documents\supplier csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0ECCD68-1038-43E9-943D-878DEFBBAFDD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78398E7-202C-4BC7-BCDD-C174E8D13939}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9660" xr2:uid="{9E7BC6C7-8E8A-4B7C-8FE3-67E2C8BF1C74}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>SupId</t>
   </si>
@@ -51,16 +51,13 @@
     <t>ALPHA OFFICE Supplies</t>
   </si>
   <si>
-    <t>Exercise</t>
-  </si>
-  <si>
-    <t>Exercise Book A4 Hardcover\r\n(120 pg)</t>
-  </si>
-  <si>
-    <t>each</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exercise Book A4 Hardcover(150pg) </t>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Clip</t>
+  </si>
+  <si>
+    <t>Clips Paper Small</t>
   </si>
 </sst>
 </file>
@@ -412,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15EA6FE1-52CC-49A0-97F3-B84668B695F8}">
-  <dimension ref="C4:I6"/>
+  <dimension ref="C4:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,42 +454,19 @@
         <v>7</v>
       </c>
       <c r="E5">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the complete import suppler and items
</commit_message>
<xml_diff>
--- a/LUSSISADTeam10Web/Content/test1.xlsx
+++ b/LUSSISADTeam10Web/Content/test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AD_Documents\supplier csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78398E7-202C-4BC7-BCDD-C174E8D13939}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CAC4B5-B4FE-4DDF-BD17-CD7E891B4B9A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9660" xr2:uid="{9E7BC6C7-8E8A-4B7C-8FE3-67E2C8BF1C74}"/>
   </bookViews>
@@ -25,20 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>SupId</t>
-  </si>
-  <si>
-    <t>ItemId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>SupName</t>
   </si>
   <si>
-    <t>CategoryName</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -51,13 +42,19 @@
     <t>ALPHA OFFICE Supplies</t>
   </si>
   <si>
-    <t>Box</t>
-  </si>
-  <si>
-    <t>Clip</t>
-  </si>
-  <si>
-    <t>Clips Paper Small</t>
+    <t>Exercise Book (10 pg)</t>
+  </si>
+  <si>
+    <t>Dozen</t>
+  </si>
+  <si>
+    <t>Exercise Book (75 pg)</t>
+  </si>
+  <si>
+    <t>Envelope White (5"x7")</t>
+  </si>
+  <si>
+    <t>Each</t>
   </si>
 </sst>
 </file>
@@ -409,64 +406,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15EA6FE1-52CC-49A0-97F3-B84668B695F8}">
-  <dimension ref="C4:I5"/>
+  <dimension ref="E4:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="24.109375" customWidth="1"/>
-    <col min="6" max="6" width="48.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" customWidth="1"/>
     <col min="7" max="8" width="5.109375" customWidth="1"/>
     <col min="9" max="9" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+    <row r="4" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="5" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G5" t="s">
         <v>6</v>
       </c>
-      <c r="I4" t="s">
-        <v>3</v>
+      <c r="H5">
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="6" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="E5">
+      <c r="G7" t="s">
         <v>6</v>
       </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" t="s">
-        <v>9</v>
+      <c r="H7">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix category and import supp item
</commit_message>
<xml_diff>
--- a/LUSSISADTeam10Web/Content/test1.xlsx
+++ b/LUSSISADTeam10Web/Content/test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AD_Documents\supplier csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CAC4B5-B4FE-4DDF-BD17-CD7E891B4B9A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633F5994-EBBD-4C81-96BB-E27E46BB5ADC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="9660" xr2:uid="{9E7BC6C7-8E8A-4B7C-8FE3-67E2C8BF1C74}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="E4:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,7 +446,7 @@
         <v>6</v>
       </c>
       <c r="H5">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="5:8" x14ac:dyDescent="0.3">

</xml_diff>